<commit_message>
ng: update bsa form
</commit_message>
<xml_diff>
--- a/ONCHO/Breeding Site Survey/Nigeria/ng_oncho_bsc_1_capture_202208.xlsx
+++ b/ONCHO/Breeding Site Survey/Nigeria/ng_oncho_bsc_1_capture_202208.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="135">
   <si>
     <t>type</t>
   </si>
@@ -58,6 +58,9 @@
     <t>choice_filter</t>
   </si>
   <si>
+    <t>read_only</t>
+  </si>
+  <si>
     <t>select_one region</t>
   </si>
   <si>
@@ -190,7 +193,7 @@
     <t>nb_collected</t>
   </si>
   <si>
-    <t>Nomber of blackflies collected</t>
+    <t>Number of blackflies collected</t>
   </si>
   <si>
     <t>select_one weather</t>
@@ -229,6 +232,9 @@
     <t>district</t>
   </si>
   <si>
+    <t>community</t>
+  </si>
+  <si>
     <t>07:00 – 08:00</t>
   </si>
   <si>
@@ -286,7 +292,7 @@
     <t>Yobe</t>
   </si>
   <si>
-    <t>Barde</t>
+    <t>Bade</t>
   </si>
   <si>
     <t>Bursari</t>
@@ -319,10 +325,7 @@
     <t>Tarmuwa</t>
   </si>
   <si>
-    <t>Yunusari</t>
-  </si>
-  <si>
-    <t>community</t>
+    <t>Yusufari</t>
   </si>
   <si>
     <t>Dagona</t>
@@ -331,7 +334,7 @@
     <t>Kaliyari</t>
   </si>
   <si>
-    <t>Rinukunu</t>
+    <t>Renukunu</t>
   </si>
   <si>
     <t>Chana</t>
@@ -340,16 +343,16 @@
     <t>Doto</t>
   </si>
   <si>
-    <t>Kermi</t>
-  </si>
-  <si>
-    <t>Abakiri</t>
-  </si>
-  <si>
-    <t>Garin Bauci</t>
-  </si>
-  <si>
-    <t>Gubber</t>
+    <t>Kurmi</t>
+  </si>
+  <si>
+    <t>Abakire</t>
+  </si>
+  <si>
+    <t>Garin Baushe</t>
+  </si>
+  <si>
+    <t>Gubana</t>
   </si>
   <si>
     <t>Madawun</t>
@@ -406,10 +409,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(2022 August) - 1. Human Landing Catches</t>
-  </si>
-  <si>
-    <t>ng_oncho_bsc_1_capture_202208</t>
+    <t>(2022 August) - 1. Human Landing Catches V2</t>
+  </si>
+  <si>
+    <t>ng_oncho_bsc_1_capture_202208_v2</t>
   </si>
   <si>
     <t>English</t>
@@ -429,10 +432,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -473,8 +476,17 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -487,17 +499,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,39 +576,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -552,13 +585,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -579,8 +605,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -592,30 +619,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -632,7 +635,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -644,7 +695,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,61 +773,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,97 +809,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -865,15 +868,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -885,6 +879,41 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -904,41 +933,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -953,151 +947,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1492,12 +1495,12 @@
   <sheetPr/>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1553,17 +1556,19 @@
       <c r="L1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="22"/>
+      <c r="M1" s="22" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:11">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="6"/>
@@ -1572,19 +1577,19 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K2" s="6"/>
     </row>
     <row r="3" s="3" customFormat="1" spans="1:12">
       <c r="A3" s="15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="9"/>
@@ -1593,25 +1598,25 @@
       <c r="H3" s="15"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" spans="1:12">
       <c r="A4" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -1619,22 +1624,22 @@
       <c r="H4" s="15"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="1" spans="1:12">
       <c r="A5" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="9"/>
@@ -1643,20 +1648,20 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="9"/>
     </row>
-    <row r="6" s="3" customFormat="1" ht="21" customHeight="1" spans="1:12">
+    <row r="6" s="3" customFormat="1" ht="21" customHeight="1" spans="1:13">
       <c r="A6" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="9"/>
@@ -1665,23 +1670,26 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="9"/>
+      <c r="M6" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:11">
       <c r="A7" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -1689,22 +1697,22 @@
       <c r="H7" s="15"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K7" s="6"/>
     </row>
     <row r="8" s="12" customFormat="1" ht="15.75" customHeight="1" spans="1:12">
       <c r="A8" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1712,20 +1720,20 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
     <row r="9" s="3" customFormat="1" spans="1:12">
       <c r="A9" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="15"/>
@@ -1734,20 +1742,20 @@
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
       <c r="J9" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
     </row>
     <row r="10" s="3" customFormat="1" spans="1:12">
       <c r="A10" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="15"/>
@@ -1755,20 +1763,20 @@
       <c r="G10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:12">
       <c r="A11" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="15"/>
@@ -1776,20 +1784,20 @@
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
     </row>
     <row r="12" s="3" customFormat="1" spans="1:12">
       <c r="A12" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="15"/>
@@ -1802,13 +1810,13 @@
     </row>
     <row r="13" s="3" customFormat="1" spans="1:12">
       <c r="A13" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="15"/>
@@ -1816,95 +1824,95 @@
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
       <c r="J13" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:12">
       <c r="A14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="H14" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I14" s="15"/>
       <c r="J14" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:12">
       <c r="A15" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="H15" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
     </row>
     <row r="16" s="3" customFormat="1" spans="1:12">
       <c r="A16" s="15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="H16" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I16" s="15"/>
       <c r="J16" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
     </row>
     <row r="17" s="3" customFormat="1" spans="1:12">
       <c r="A17" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="H17" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I17" s="15"/>
       <c r="J17" s="6"/>
@@ -1913,7 +1921,7 @@
     </row>
     <row r="18" s="3" customFormat="1" spans="1:12">
       <c r="A18" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -1927,10 +1935,10 @@
     </row>
     <row r="19" s="3" customFormat="1" spans="1:12">
       <c r="A19" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -1944,10 +1952,10 @@
     </row>
     <row r="20" s="3" customFormat="1" spans="1:12">
       <c r="A20" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -1986,10 +1994,10 @@
   <sheetPr/>
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="$A35:$XFD35"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="$A59:$XFD81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -2003,7 +2011,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -2012,703 +2020,705 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E35" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E36" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E37" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E38" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E39" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C42" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E42" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E43" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E44" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E45" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C46" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E46" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E47" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C48" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E48" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C49" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E49" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C50" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E50" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C51" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E51" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B52" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C52" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E52" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C53" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E53" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C54" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E54" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B55" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C55" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E55" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" t="s">
+        <v>123</v>
+      </c>
+      <c r="C56" t="s">
+        <v>123</v>
+      </c>
+      <c r="E56" t="s">
         <v>100</v>
-      </c>
-      <c r="B56" t="s">
-        <v>122</v>
-      </c>
-      <c r="C56" t="s">
-        <v>122</v>
-      </c>
-      <c r="E56" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C57" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E57" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2727,42 +2737,42 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A20" sqref="$A20:$XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="44.1111111111111" customWidth="1"/>
-    <col min="2" max="2" width="30.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="34.7777777777778" customWidth="1"/>
     <col min="3" max="3" width="11.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C2">
         <v>20210625</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2775,377 +2785,441 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="6.22222222222222" customWidth="1"/>
     <col min="2" max="2" width="11.8888888888889" customWidth="1"/>
-    <col min="3" max="3" width="12.4444444444444" customWidth="1"/>
-    <col min="6" max="6" width="6.22222222222222" customWidth="1"/>
-    <col min="7" max="7" width="11.8888888888889" customWidth="1"/>
+    <col min="3" max="4" width="12.4444444444444" customWidth="1"/>
+    <col min="7" max="7" width="6.22222222222222" customWidth="1"/>
+    <col min="8" max="8" width="11.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2">
         <v>101</v>
       </c>
-      <c r="D2"/>
-      <c r="F2" t="s">
-        <v>87</v>
-      </c>
       <c r="G2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>89</v>
+      </c>
+      <c r="H2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3">
         <v>102</v>
       </c>
-      <c r="D3"/>
-      <c r="F3" t="s">
-        <v>87</v>
-      </c>
       <c r="G3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4">
         <v>103</v>
       </c>
-      <c r="D4"/>
-      <c r="F4" t="s">
-        <v>87</v>
-      </c>
       <c r="G4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>89</v>
+      </c>
+      <c r="H4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5">
         <v>104</v>
       </c>
-      <c r="D5"/>
-      <c r="F5" t="s">
-        <v>87</v>
-      </c>
       <c r="G5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>89</v>
+      </c>
+      <c r="H5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6">
         <v>105</v>
       </c>
-      <c r="D6"/>
-      <c r="F6" t="s">
-        <v>87</v>
-      </c>
       <c r="G6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" t="s">
-        <v>90</v>
-      </c>
       <c r="C7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7">
         <v>106</v>
       </c>
-      <c r="D7"/>
-      <c r="F7" t="s">
-        <v>87</v>
-      </c>
       <c r="G7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" t="s">
-        <v>91</v>
-      </c>
       <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8">
         <v>107</v>
       </c>
-      <c r="D8"/>
-      <c r="F8" t="s">
-        <v>87</v>
-      </c>
       <c r="G8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9">
+        <v>108</v>
+      </c>
+      <c r="G9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10">
+        <v>109</v>
+      </c>
+      <c r="G10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11">
+        <v>110</v>
+      </c>
+      <c r="G11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12">
+        <v>111</v>
+      </c>
+      <c r="G12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9"/>
-      <c r="F9" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="C13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13">
+        <v>112</v>
+      </c>
+      <c r="G13" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D10"/>
-      <c r="F10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="C14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D11"/>
-      <c r="F11" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="C16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" t="s">
-        <v>111</v>
-      </c>
-      <c r="D12"/>
-      <c r="F12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="C17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" t="s">
-        <v>112</v>
-      </c>
-      <c r="D13"/>
-      <c r="F13" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" t="s">
-        <v>93</v>
-      </c>
-      <c r="C14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21" t="s">
-        <v>97</v>
-      </c>
       <c r="C21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22">
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23">
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24">
         <v>123</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C$1:C$1048576">
+  <sortState ref="B2:C24">
+    <sortCondition ref="B2:B24"/>
+    <sortCondition ref="C2:C24"/>
+  </sortState>
+  <conditionalFormatting sqref="C$1:D$1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>